<commit_message>
Merged remote main and added updated Excel files
</commit_message>
<xml_diff>
--- a/Matningsdata.xlsx
+++ b/Matningsdata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://skanska-my.sharepoint.com/personal/erica_carneiro_skanska_se/Documents/ECa/Täby Park/GWR/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="118" documentId="8_{EA5E93D8-7595-4ED3-9CF0-C8CEEB1F7833}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BE24C023-3E61-4C31-8080-449CD0A8F17E}"/>
+  <xr:revisionPtr revIDLastSave="122" documentId="8_{EA5E93D8-7595-4ED3-9CF0-C8CEEB1F7833}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{40DE028A-CC7B-4748-9929-1EB971FA93CD}"/>
   <bookViews>
-    <workbookView xWindow="49755" yWindow="2730" windowWidth="16920" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Kostnadsfordelning" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Månadsvisa rör</t>
   </si>
@@ -69,15 +69,6 @@
   </si>
   <si>
     <t>Fakturtotal (kr):</t>
-  </si>
-  <si>
-    <t>Rörmängd</t>
-  </si>
-  <si>
-    <t>ID</t>
-  </si>
-  <si>
-    <t>TPAB</t>
   </si>
 </sst>
 </file>
@@ -233,7 +224,7 @@
     <cellStyle name="Beräkning" xfId="1" builtinId="22"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="11">
+  <dxfs count="9">
     <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
       <border diagonalUp="0" diagonalDown="0">
@@ -308,60 +299,6 @@
       </border>
     </dxf>
     <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color auto="1"/>
@@ -460,17 +397,11 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{D088FFEC-C2A4-4E16-A07E-64961FCB02D5}" name="Tabell3" displayName="Tabell3" ref="A1:H7" totalsRowShown="0" headerRowDxfId="10" headerRowBorderDxfId="9" tableBorderDxfId="8">
-  <autoFilter ref="A1:H7" xr:uid="{D088FFEC-C2A4-4E16-A07E-64961FCB02D5}"/>
-  <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{6F5211C7-8D0C-4F89-8B2C-2B1CC3657CBA}" name="DP (TPAB)" dataDxfId="7"/>
-    <tableColumn id="8" xr3:uid="{FA597EB4-DEDF-407A-9F07-62769414D5C0}" name="ID" dataDxfId="6"/>
-    <tableColumn id="7" xr3:uid="{B7F6B325-97A4-4ACD-9CEA-3E13E034AD97}" name="Rörmängd" dataDxfId="5"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{D088FFEC-C2A4-4E16-A07E-64961FCB02D5}" name="Tabell3" displayName="Tabell3" ref="A1:F7" totalsRowShown="0" headerRowDxfId="8" headerRowBorderDxfId="7" tableBorderDxfId="6">
+  <autoFilter ref="A1:F7" xr:uid="{D088FFEC-C2A4-4E16-A07E-64961FCB02D5}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{6F5211C7-8D0C-4F89-8B2C-2B1CC3657CBA}" name="DP (TPAB)" dataDxfId="5"/>
     <tableColumn id="2" xr3:uid="{D824F042-C707-4AAB-AC65-3D4F0C0B94D1}" name="Månadsvisa rör" dataDxfId="4"/>
     <tableColumn id="3" xr3:uid="{F705E739-96CB-4636-A544-4950FADE0C4A}" name="Kvartalsvisa rör" dataDxfId="3"/>
     <tableColumn id="4" xr3:uid="{FE1F902C-B8F7-4C12-A1D1-57C506FDE6E0}" name="Årsmätningar" dataDxfId="2"/>
@@ -768,210 +699,167 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15" style="5" customWidth="1"/>
-    <col min="4" max="4" width="24.5703125" style="5" customWidth="1"/>
-    <col min="5" max="5" width="26.140625" style="5" customWidth="1"/>
-    <col min="6" max="6" width="17.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.140625" style="5"/>
-    <col min="8" max="8" width="16.140625" style="5" customWidth="1"/>
-    <col min="9" max="9" width="17.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="9.140625" style="5"/>
+    <col min="2" max="2" width="24.5703125" style="5" customWidth="1"/>
+    <col min="3" max="3" width="26.140625" style="5" customWidth="1"/>
+    <col min="4" max="4" width="17.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" style="5"/>
+    <col min="6" max="6" width="16.140625" style="5" customWidth="1"/>
+    <col min="7" max="7" width="17.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>10</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="D1" s="9" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="F1" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="G1" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="10" t="s">
+      <c r="F1" s="10" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2" s="2">
+      <c r="B2" s="1">
         <v>2</v>
       </c>
+      <c r="C2" s="1">
+        <v>0</v>
+      </c>
       <c r="D2" s="1">
-        <v>2</v>
+        <f>B2*12+C2*4</f>
+        <v>24</v>
       </c>
       <c r="E2" s="1">
-        <v>0</v>
-      </c>
-      <c r="F2" s="1">
-        <f>D2*12+E2*4</f>
-        <v>24</v>
-      </c>
-      <c r="G2" s="1">
-        <f>F2/SUM($F$2:$F$6)</f>
+        <f>D2/SUM($D$2:$D$6)</f>
         <v>5.5045871559633031E-2</v>
       </c>
-      <c r="H2" s="3">
-        <f>D$7*G2</f>
+      <c r="F2" s="3">
+        <f>B$7*E2</f>
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C3" s="2">
-        <v>7</v>
+      <c r="B3" s="1">
+        <v>6</v>
+      </c>
+      <c r="C3" s="1">
+        <v>1</v>
       </c>
       <c r="D3" s="1">
-        <v>6</v>
+        <f t="shared" ref="D3:D6" si="0">B3*12+C3*4</f>
+        <v>76</v>
       </c>
       <c r="E3" s="1">
-        <v>1</v>
-      </c>
-      <c r="F3" s="1">
-        <f t="shared" ref="F3:F6" si="0">D3*12+E3*4</f>
-        <v>76</v>
-      </c>
-      <c r="G3" s="1">
-        <f>F3/SUM($F$2:$F$6)</f>
+        <f>D3/SUM($D$2:$D$6)</f>
         <v>0.1743119266055046</v>
       </c>
-      <c r="H3" s="3">
-        <f>D$7*G3</f>
+      <c r="F3" s="3">
+        <f>B$7*E3</f>
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" s="2">
+      <c r="B4" s="1">
         <v>13</v>
       </c>
+      <c r="C4" s="1">
+        <v>0</v>
+      </c>
       <c r="D4" s="1">
-        <v>13</v>
-      </c>
-      <c r="E4" s="1">
-        <v>0</v>
-      </c>
-      <c r="F4" s="1">
         <f t="shared" si="0"/>
         <v>156</v>
       </c>
-      <c r="G4" s="1">
-        <f>F4/SUM($F$2:$F$6)</f>
+      <c r="E4" s="1">
+        <f>D4/SUM($D$2:$D$6)</f>
         <v>0.3577981651376147</v>
       </c>
-      <c r="H4" s="3">
-        <f>D$7*G4</f>
+      <c r="F4" s="3">
+        <f>B$7*E4</f>
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" s="2">
+      <c r="B5" s="1">
         <v>12</v>
       </c>
+      <c r="C5" s="1">
+        <v>0</v>
+      </c>
       <c r="D5" s="1">
-        <v>12</v>
-      </c>
-      <c r="E5" s="1">
-        <v>0</v>
-      </c>
-      <c r="F5" s="1">
         <f t="shared" si="0"/>
         <v>144</v>
       </c>
-      <c r="G5" s="1">
-        <f>F5/SUM($F$2:$F$6)</f>
+      <c r="E5" s="1">
+        <f>D5/SUM($D$2:$D$6)</f>
         <v>0.33027522935779818</v>
       </c>
-      <c r="H5" s="3">
-        <f>D$7*G5</f>
+      <c r="F5" s="3">
+        <f>B$7*E5</f>
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" s="2">
+      <c r="B6" s="1">
         <v>3</v>
       </c>
+      <c r="C6" s="1">
+        <v>0</v>
+      </c>
       <c r="D6" s="1">
-        <v>3</v>
-      </c>
-      <c r="E6" s="1">
-        <v>0</v>
-      </c>
-      <c r="F6" s="1">
         <f t="shared" si="0"/>
         <v>36</v>
       </c>
-      <c r="G6" s="1">
-        <f>F6/SUM($F$2:$F$6)</f>
+      <c r="E6" s="1">
+        <f>D6/SUM($D$2:$D$6)</f>
         <v>8.2568807339449546E-2</v>
       </c>
-      <c r="H6" s="3">
-        <f>D$7*G6</f>
+      <c r="F6" s="3">
+        <f>B$7*E6</f>
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="7"/>
-      <c r="C7" s="7">
-        <f>SUM(C2:C6)</f>
-        <v>37</v>
-      </c>
-      <c r="D7" s="4">
-        <v>0</v>
-      </c>
-      <c r="H7" s="8"/>
+      <c r="B7" s="4">
+        <v>0</v>
+      </c>
+      <c r="F7" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update Matningsdata.xlsx for Streamlit app
</commit_message>
<xml_diff>
--- a/Matningsdata.xlsx
+++ b/Matningsdata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://skanska-my.sharepoint.com/personal/erica_carneiro_skanska_se/Documents/ECa/Täby Park/GWR/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="122" documentId="8_{EA5E93D8-7595-4ED3-9CF0-C8CEEB1F7833}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{40DE028A-CC7B-4748-9929-1EB971FA93CD}"/>
+  <xr:revisionPtr revIDLastSave="128" documentId="8_{EA5E93D8-7595-4ED3-9CF0-C8CEEB1F7833}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2455653E-01C3-47A0-B5F7-74CDF0474700}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Månadsvisa rör</t>
   </si>
@@ -66,29 +66,19 @@
   </si>
   <si>
     <t>DP (TPAB)</t>
-  </si>
-  <si>
-    <t>Fakturtotal (kr):</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -105,7 +95,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -114,18 +104,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -136,7 +115,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -161,21 +140,6 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color auto="1"/>
       </left>
       <right style="thin">
@@ -188,40 +152,31 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Beräkning" xfId="1" builtinId="22"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="9">
@@ -398,8 +353,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{D088FFEC-C2A4-4E16-A07E-64961FCB02D5}" name="Tabell3" displayName="Tabell3" ref="A1:F7" totalsRowShown="0" headerRowDxfId="8" headerRowBorderDxfId="7" tableBorderDxfId="6">
-  <autoFilter ref="A1:F7" xr:uid="{D088FFEC-C2A4-4E16-A07E-64961FCB02D5}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{D088FFEC-C2A4-4E16-A07E-64961FCB02D5}" name="Tabell3" displayName="Tabell3" ref="A1:F6" totalsRowShown="0" headerRowDxfId="8" headerRowBorderDxfId="7" tableBorderDxfId="6">
+  <autoFilter ref="A1:F6" xr:uid="{D088FFEC-C2A4-4E16-A07E-64961FCB02D5}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{6F5211C7-8D0C-4F89-8B2C-2B1CC3657CBA}" name="DP (TPAB)" dataDxfId="5"/>
     <tableColumn id="2" xr3:uid="{D824F042-C707-4AAB-AC65-3D4F0C0B94D1}" name="Månadsvisa rör" dataDxfId="4"/>
@@ -699,41 +654,41 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.5703125" style="5" customWidth="1"/>
-    <col min="3" max="3" width="26.140625" style="5" customWidth="1"/>
-    <col min="4" max="4" width="17.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" style="5"/>
-    <col min="6" max="6" width="16.140625" style="5" customWidth="1"/>
-    <col min="7" max="7" width="17.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="5"/>
+    <col min="1" max="1" width="15" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.5703125" style="4" customWidth="1"/>
+    <col min="3" max="3" width="26.140625" style="4" customWidth="1"/>
+    <col min="4" max="4" width="17.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" style="4"/>
+    <col min="6" max="6" width="16.140625" style="4" customWidth="1"/>
+    <col min="7" max="7" width="17.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="F1" s="7" t="s">
         <v>9</v>
       </c>
     </row>
@@ -755,13 +710,13 @@
         <f>D2/SUM($D$2:$D$6)</f>
         <v>5.5045871559633031E-2</v>
       </c>
-      <c r="F2" s="3">
-        <f>B$7*E2</f>
-        <v>0</v>
+      <c r="F2" s="3" t="e">
+        <f>#REF!*E2</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="11" t="s">
+      <c r="A3" s="8" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="1">
@@ -778,13 +733,13 @@
         <f>D3/SUM($D$2:$D$6)</f>
         <v>0.1743119266055046</v>
       </c>
-      <c r="F3" s="3">
-        <f>B$7*E3</f>
-        <v>0</v>
+      <c r="F3" s="3" t="e">
+        <f>#REF!*E3</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="11" t="s">
+      <c r="A4" s="8" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="1">
@@ -801,13 +756,13 @@
         <f>D4/SUM($D$2:$D$6)</f>
         <v>0.3577981651376147</v>
       </c>
-      <c r="F4" s="3">
-        <f>B$7*E4</f>
-        <v>0</v>
+      <c r="F4" s="3" t="e">
+        <f>#REF!*E4</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="11" t="s">
+      <c r="A5" s="8" t="s">
         <v>7</v>
       </c>
       <c r="B5" s="1">
@@ -824,13 +779,13 @@
         <f>D5/SUM($D$2:$D$6)</f>
         <v>0.33027522935779818</v>
       </c>
-      <c r="F5" s="3">
-        <f>B$7*E5</f>
-        <v>0</v>
+      <c r="F5" s="3" t="e">
+        <f>#REF!*E5</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="11" t="s">
+      <c r="A6" s="8" t="s">
         <v>8</v>
       </c>
       <c r="B6" s="1">
@@ -847,19 +802,10 @@
         <f>D6/SUM($D$2:$D$6)</f>
         <v>8.2568807339449546E-2</v>
       </c>
-      <c r="F6" s="3">
-        <f>B$7*E6</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" s="4">
-        <v>0</v>
-      </c>
-      <c r="F7" s="8"/>
+      <c r="F6" s="3" t="e">
+        <f>#REF!*E6</f>
+        <v>#REF!</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>